<commit_message>
edit excel file input
</commit_message>
<xml_diff>
--- a/input/dtcs_definition.xlsx
+++ b/input/dtcs_definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Source\automation\oem-service-compare-data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA6F078-C82E-485B-9008-12A66297E6BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C385681-3C09-44CF-8A5C-53D7B4512AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28908" yWindow="-60" windowWidth="29016" windowHeight="15696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -454,7 +454,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>